<commit_message>
Create Spring0 folder for next week presetation - Yunwei
Create Spring0 folder for next week presetation - Yunwei
</commit_message>
<xml_diff>
--- a/Doc/ICSI518_ Team_WorkLists.xlsx
+++ b/Doc/ICSI518_ Team_WorkLists.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0DDEE5-EE44-43C5-BED8-9B77CCFF7728}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB14392-0762-4EC1-B431-232F364C8AE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Role</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,14 +166,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Seller Module Requirements Specification,Backlog,Architecture,Database Desgin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Buyer Module Requirements Specification,Backlog,Architecture,Database Desgin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PPT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -185,17 +177,48 @@
   <si>
     <t>Sreekar,
 Akshay</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Main Page Requirements Specification,Backlog,Architecture,Database Desgin;
-Admin Module Requirements Specification,Backlog,Architecture,Database Desgin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Brian Juan
 Hemanshu, Joshi
 Ashita, Kalidindi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The completed product backlog, with story points and all stories ordered</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Buyer
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High-level software architecture</t>
+  </si>
+  <si>
+    <t>Tools and technologies to be used</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buyer Module Requirements Specification,Backlog,Architecture,story points and all stories ordered,Tools and technologies to be used</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seller Module Requirements Specification,Backlog,Architecture,story points and all stories ordered,Tools and technologies to be used</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All members</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main WebSite and Admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main WebSite and  Admin Module Requirements Specification,Backlog,Architecture,story points and all stories ordered, Tools and technologies to be used</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -560,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -575,193 +598,319 @@
     <col min="5" max="5" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
+    <row r="30" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>